<commit_message>
initiating push part 2
</commit_message>
<xml_diff>
--- a/sfs_data/USFS_data-EK.xlsx
+++ b/sfs_data/USFS_data-EK.xlsx
@@ -838,13 +838,13 @@
   <dimension ref="A1:AMJ46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="G25:H30"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.21"/>
@@ -2427,7 +2427,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G25:H30 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>